<commit_message>
more slight fixes to matlab
</commit_message>
<xml_diff>
--- a/graphs/pathRand_1000_u11/plot_errors.xlsx
+++ b/graphs/pathRand_1000_u11/plot_errors.xlsx
@@ -1063,7 +1063,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6525-44DA-AB5F-DF3CEC83CF6C}"/>
+              <c16:uniqueId val="{00000000-D82A-4D02-9812-6EA49DA35274}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1702,7 +1702,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-6525-44DA-AB5F-DF3CEC83CF6C}"/>
+              <c16:uniqueId val="{00000001-D82A-4D02-9812-6EA49DA35274}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2341,7 +2341,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-6525-44DA-AB5F-DF3CEC83CF6C}"/>
+              <c16:uniqueId val="{00000002-D82A-4D02-9812-6EA49DA35274}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2980,7 +2980,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-6525-44DA-AB5F-DF3CEC83CF6C}"/>
+              <c16:uniqueId val="{00000003-D82A-4D02-9812-6EA49DA35274}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3538,7 +3538,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-56F9-45C5-8FEE-85A52FAFE334}"/>
+              <c16:uniqueId val="{00000000-7EDA-47E1-AD94-828DA041737F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3880,7 +3880,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-56F9-45C5-8FEE-85A52FAFE334}"/>
+              <c16:uniqueId val="{00000001-7EDA-47E1-AD94-828DA041737F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4222,7 +4222,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-56F9-45C5-8FEE-85A52FAFE334}"/>
+              <c16:uniqueId val="{00000002-7EDA-47E1-AD94-828DA041737F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4564,7 +4564,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-56F9-45C5-8FEE-85A52FAFE334}"/>
+              <c16:uniqueId val="{00000003-7EDA-47E1-AD94-828DA041737F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4906,7 +4906,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-56F9-45C5-8FEE-85A52FAFE334}"/>
+              <c16:uniqueId val="{00000004-7EDA-47E1-AD94-828DA041737F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5248,7 +5248,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-56F9-45C5-8FEE-85A52FAFE334}"/>
+              <c16:uniqueId val="{00000005-7EDA-47E1-AD94-828DA041737F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5592,7 +5592,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-56F9-45C5-8FEE-85A52FAFE334}"/>
+              <c16:uniqueId val="{00000006-7EDA-47E1-AD94-828DA041737F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5936,7 +5936,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-56F9-45C5-8FEE-85A52FAFE334}"/>
+              <c16:uniqueId val="{00000007-7EDA-47E1-AD94-828DA041737F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7863,21 +7863,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>250031</xdr:colOff>
-      <xdr:row>185</xdr:row>
-      <xdr:rowOff>83343</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>288131</xdr:colOff>
-      <xdr:row>200</xdr:row>
-      <xdr:rowOff>111918</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -7899,20 +7901,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>502442</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>130968</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>540542</xdr:colOff>
-      <xdr:row>87</xdr:row>
-      <xdr:rowOff>159543</xdr:rowOff>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -8286,8 +8290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:M200"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -38332,7 +38336,7 @@
   <dimension ref="A1:Q401"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:Q2"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>